<commit_message>
v8 ipynb some more analysis of shops
</commit_message>
<xml_diff>
--- a/data_output/shops_augmented sales analysis with fig.xlsx
+++ b/data_output/shops_augmented sales analysis with fig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgaid\Google Drive\Colab Notebooks\NRUHSE_2_Kaggle_Coursera\final\Kag\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CF4B2D21-9D5F-4F96-87A8-2C7A7B3D6329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DAE82ACC-5A01-4DE1-AB39-15FA0C4B9F7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="284">
   <si>
     <t>shop_name</t>
   </si>
@@ -860,6 +860,18 @@
   </si>
   <si>
     <t>Not insignificant sales between the spikes, but the 3 spikes dominate by far</t>
+  </si>
+  <si>
+    <t>small bumps at 365/730</t>
+  </si>
+  <si>
+    <t>2, 4, 14, 18, 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17, 18, 36, 37, 38, 48, </t>
+  </si>
+  <si>
+    <t>Correlation evaluated by month, instead of as a whole:</t>
   </si>
 </sst>
 </file>
@@ -1466,6 +1478,138 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>277370</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>744</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85B22F63-6DBC-42B8-A6EF-047604B48B8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14859000" y="11811000"/>
+          <a:ext cx="8202170" cy="5334744"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>421201</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>162559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A6F9A5-DE38-4176-A40B-7EEA2E0BDA45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14859000" y="17526000"/>
+          <a:ext cx="15051601" cy="4544059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>29685</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>105295</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F412A25B-5FE2-49F8-AECF-94CFB6F5B6C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14859000" y="22669500"/>
+          <a:ext cx="7954485" cy="3724795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1766,10 +1910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D38" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2963,7 +3107,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2998,7 +3142,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -3030,7 +3174,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -3062,7 +3206,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>103</v>
       </c>
@@ -3100,7 +3244,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -3135,7 +3279,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -3167,7 +3311,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -3205,7 +3349,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -3240,7 +3384,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -3278,7 +3422,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -3310,7 +3454,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -3342,7 +3486,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>123</v>
       </c>
@@ -3374,7 +3518,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -3408,8 +3552,11 @@
       <c r="K45" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -3441,7 +3588,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>131</v>
       </c>
@@ -3473,7 +3620,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -3503,6 +3650,9 @@
       </c>
       <c r="K48" t="s">
         <v>256</v>
+      </c>
+      <c r="O48" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3731,14 +3881,11 @@
       <c r="H55" t="b">
         <v>1</v>
       </c>
-      <c r="I55" t="s">
-        <v>276</v>
-      </c>
       <c r="J55" t="s">
         <v>241</v>
       </c>
       <c r="K55" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3767,16 +3914,13 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J56" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="K56" t="s">
-        <v>277</v>
-      </c>
-      <c r="L56" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3804,6 +3948,18 @@
       <c r="H57" t="b">
         <v>1</v>
       </c>
+      <c r="I57" t="s">
+        <v>278</v>
+      </c>
+      <c r="J57" t="s">
+        <v>239</v>
+      </c>
+      <c r="K57" t="s">
+        <v>277</v>
+      </c>
+      <c r="L57" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -3830,6 +3986,12 @@
       <c r="H58" t="b">
         <v>1</v>
       </c>
+      <c r="J58" t="s">
+        <v>241</v>
+      </c>
+      <c r="K58" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -3856,6 +4018,12 @@
       <c r="H59" t="b">
         <v>1</v>
       </c>
+      <c r="J59" t="s">
+        <v>242</v>
+      </c>
+      <c r="K59" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -3882,6 +4050,12 @@
       <c r="H60" t="b">
         <v>1</v>
       </c>
+      <c r="J60" t="s">
+        <v>241</v>
+      </c>
+      <c r="K60" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -3907,6 +4081,17 @@
       </c>
       <c r="H61" t="b">
         <v>1</v>
+      </c>
+      <c r="J61" t="s">
+        <v>241</v>
+      </c>
+      <c r="K61" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="119" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M119" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>